<commit_message>
Added Adobe Premiere Project. Includes footage and some edit/placement of footage.
</commit_message>
<xml_diff>
--- a/Documentation/Footage Requirements.xlsx
+++ b/Documentation/Footage Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -21,7 +21,34 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Candidate Links:
+https://www.youtube.com/watch?v=A42mHv2pqsY
+https://www.youtube.com/watch?v=IWU5Apfu3gQ
+https://www.youtube.com/watch?v=Desl_yeM6DA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,32 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Candidate Links:
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -745,7 +747,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +782,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -991,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>